<commit_message>
Diseño vistas - pagina en general
Se realizaron cambios en las interfaces de toda la pagina en general
</commit_message>
<xml_diff>
--- a/sgtcis/app/Files/plantilla_docentes.xlsx
+++ b/sgtcis/app/Files/plantilla_docentes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4200" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="5400" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
   <si>
     <t>password</t>
   </si>
@@ -189,16 +189,7 @@
     <t>NA</t>
   </si>
   <si>
-    <t>paralelo_a</t>
-  </si>
-  <si>
-    <t>paralelo_b</t>
-  </si>
-  <si>
-    <t>paralelo_c</t>
-  </si>
-  <si>
-    <t>paralelo_d</t>
+    <t>paralelo</t>
   </si>
 </sst>
 </file>
@@ -243,10 +234,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -528,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +536,7 @@
     <col min="8" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -572,19 +562,10 @@
         <v>56</v>
       </c>
       <c r="I1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K1" t="s">
-        <v>59</v>
-      </c>
-      <c r="L1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -606,23 +587,14 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>55</v>
       </c>
       <c r="I2" t="s">
         <v>55</v>
       </c>
-      <c r="J2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" t="s">
-        <v>55</v>
-      </c>
-      <c r="L2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -644,23 +616,14 @@
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" t="s">
         <v>55</v>
       </c>
       <c r="I3" t="s">
         <v>55</v>
       </c>
-      <c r="J3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -682,23 +645,14 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" t="s">
         <v>55</v>
       </c>
       <c r="I4" t="s">
         <v>55</v>
       </c>
-      <c r="J4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K4" t="s">
-        <v>55</v>
-      </c>
-      <c r="L4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -720,23 +674,14 @@
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" t="s">
         <v>55</v>
       </c>
       <c r="I5" t="s">
         <v>55</v>
       </c>
-      <c r="J5" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" t="s">
-        <v>55</v>
-      </c>
-      <c r="L5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -758,23 +703,14 @@
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" t="s">
         <v>55</v>
       </c>
       <c r="I6" t="s">
         <v>55</v>
       </c>
-      <c r="J6" t="s">
-        <v>55</v>
-      </c>
-      <c r="K6" t="s">
-        <v>55</v>
-      </c>
-      <c r="L6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -796,23 +732,14 @@
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" t="s">
         <v>55</v>
       </c>
       <c r="I7" t="s">
         <v>55</v>
       </c>
-      <c r="J7" t="s">
-        <v>55</v>
-      </c>
-      <c r="K7" t="s">
-        <v>55</v>
-      </c>
-      <c r="L7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -834,23 +761,14 @@
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" t="s">
         <v>55</v>
       </c>
       <c r="I8" t="s">
         <v>55</v>
       </c>
-      <c r="J8" t="s">
-        <v>55</v>
-      </c>
-      <c r="K8" t="s">
-        <v>55</v>
-      </c>
-      <c r="L8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -872,23 +790,14 @@
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" t="s">
         <v>55</v>
       </c>
       <c r="I9" t="s">
         <v>55</v>
       </c>
-      <c r="J9" t="s">
-        <v>55</v>
-      </c>
-      <c r="K9" t="s">
-        <v>55</v>
-      </c>
-      <c r="L9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -910,23 +819,14 @@
       <c r="G10">
         <v>1</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" t="s">
         <v>55</v>
       </c>
       <c r="I10" t="s">
         <v>55</v>
       </c>
-      <c r="J10" t="s">
-        <v>55</v>
-      </c>
-      <c r="K10" t="s">
-        <v>55</v>
-      </c>
-      <c r="L10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -948,23 +848,14 @@
       <c r="G11">
         <v>1</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" t="s">
         <v>55</v>
       </c>
       <c r="I11" t="s">
         <v>55</v>
       </c>
-      <c r="J11" t="s">
-        <v>55</v>
-      </c>
-      <c r="K11" t="s">
-        <v>55</v>
-      </c>
-      <c r="L11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -986,23 +877,14 @@
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" t="s">
         <v>55</v>
       </c>
       <c r="I12" t="s">
         <v>55</v>
       </c>
-      <c r="J12" t="s">
-        <v>55</v>
-      </c>
-      <c r="K12" t="s">
-        <v>55</v>
-      </c>
-      <c r="L12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -1024,19 +906,10 @@
       <c r="G13">
         <v>1</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" t="s">
         <v>55</v>
       </c>
       <c r="I13" t="s">
-        <v>55</v>
-      </c>
-      <c r="J13" t="s">
-        <v>55</v>
-      </c>
-      <c r="K13" t="s">
-        <v>55</v>
-      </c>
-      <c r="L13" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>